<commit_message>
enter data thru AvF trial 3
</commit_message>
<xml_diff>
--- a/data/cannibalCounts.xlsx
+++ b/data/cannibalCounts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/augkd/Documents/GitHub/forbesiVsrubens/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F556DDA7-77DB-6941-9548-80F9EF3C6025}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B9FDF81-1639-CF4D-BAD9-F76B5BDC8262}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9020" yWindow="500" windowWidth="27640" windowHeight="16940" xr2:uid="{42AF5F07-34B4-EB41-A592-078703C6BD40}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="14">
   <si>
     <t>Experiment</t>
   </si>
@@ -66,6 +66,18 @@
   </si>
   <si>
     <t>Ar</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>"Potential peripheral cannibalism among glowers"</t>
+  </si>
+  <si>
+    <t>"Big guy was eating the third glower"</t>
+  </si>
+  <si>
+    <t>"Cannibalism pileup apparently on non-glower"</t>
   </si>
 </sst>
 </file>
@@ -118,6 +130,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -437,15 +453,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD071DE8-017B-EB4B-963A-ABFFC1C9D0E0}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:H58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -467,8 +483,11 @@
       <c r="G1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -487,8 +506,11 @@
       <c r="F2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -507,8 +529,11 @@
       <c r="F3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -527,8 +552,11 @@
       <c r="F4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -547,8 +575,11 @@
       <c r="F5" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -567,8 +598,11 @@
       <c r="F6" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -587,8 +621,11 @@
       <c r="F7" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -607,8 +644,11 @@
       <c r="F8" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -627,8 +667,11 @@
       <c r="F9" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -647,8 +690,11 @@
       <c r="F10" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -667,8 +713,11 @@
       <c r="F11" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -687,8 +736,11 @@
       <c r="F12" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -707,8 +759,11 @@
       <c r="F13" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -727,8 +782,11 @@
       <c r="F14" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -747,8 +805,11 @@
       <c r="F15" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -767,8 +828,11 @@
       <c r="F16" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -787,8 +851,11 @@
       <c r="F17" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -807,8 +874,11 @@
       <c r="F18" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -827,8 +897,11 @@
       <c r="F19" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>6</v>
       </c>
@@ -847,8 +920,11 @@
       <c r="F20" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>6</v>
       </c>
@@ -866,6 +942,675 @@
       </c>
       <c r="F21" t="b">
         <v>1</v>
+      </c>
+      <c r="G21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>5</v>
+      </c>
+      <c r="F22" t="b">
+        <v>0</v>
+      </c>
+      <c r="G22" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>5</v>
+      </c>
+      <c r="F23" t="b">
+        <v>0</v>
+      </c>
+      <c r="G23" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24">
+        <v>2</v>
+      </c>
+      <c r="E24">
+        <v>4</v>
+      </c>
+      <c r="F24" t="b">
+        <v>0</v>
+      </c>
+      <c r="G24" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25">
+        <v>2</v>
+      </c>
+      <c r="D25">
+        <v>3</v>
+      </c>
+      <c r="E25">
+        <v>3</v>
+      </c>
+      <c r="F25" t="b">
+        <v>0</v>
+      </c>
+      <c r="G25" t="b">
+        <v>0</v>
+      </c>
+      <c r="H25" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26">
+        <v>4</v>
+      </c>
+      <c r="E26">
+        <v>2</v>
+      </c>
+      <c r="F26" t="b">
+        <v>0</v>
+      </c>
+      <c r="G26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
+      </c>
+      <c r="D27">
+        <v>5</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27" t="b">
+        <v>0</v>
+      </c>
+      <c r="G27" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="D28">
+        <v>6</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28" t="b">
+        <v>0</v>
+      </c>
+      <c r="G28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29">
+        <v>7</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29" t="b">
+        <v>0</v>
+      </c>
+      <c r="G29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30">
+        <v>2</v>
+      </c>
+      <c r="D30">
+        <v>8</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30" t="b">
+        <v>0</v>
+      </c>
+      <c r="G30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
+      <c r="D31">
+        <v>9</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31" t="b">
+        <v>1</v>
+      </c>
+      <c r="G31" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32">
+        <v>2</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>5</v>
+      </c>
+      <c r="F32" t="b">
+        <v>0</v>
+      </c>
+      <c r="G32" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33">
+        <v>2</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <v>4</v>
+      </c>
+      <c r="F33" t="b">
+        <v>0</v>
+      </c>
+      <c r="G33" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34">
+        <v>2</v>
+      </c>
+      <c r="D34">
+        <v>2</v>
+      </c>
+      <c r="E34">
+        <v>3</v>
+      </c>
+      <c r="F34" t="b">
+        <v>0</v>
+      </c>
+      <c r="G34" t="b">
+        <v>1</v>
+      </c>
+      <c r="H34" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35">
+        <v>2</v>
+      </c>
+      <c r="D35">
+        <v>3</v>
+      </c>
+      <c r="E35">
+        <v>2</v>
+      </c>
+      <c r="F35" t="b">
+        <v>0</v>
+      </c>
+      <c r="G35" t="b">
+        <v>1</v>
+      </c>
+      <c r="H35" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36" t="s">
+        <v>9</v>
+      </c>
+      <c r="C36">
+        <v>2</v>
+      </c>
+      <c r="D36">
+        <v>4</v>
+      </c>
+      <c r="E36">
+        <v>2</v>
+      </c>
+      <c r="F36" t="b">
+        <v>0</v>
+      </c>
+      <c r="G36" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37" t="s">
+        <v>9</v>
+      </c>
+      <c r="C37">
+        <v>2</v>
+      </c>
+      <c r="D37">
+        <v>5</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37" t="b">
+        <v>0</v>
+      </c>
+      <c r="G37" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>6</v>
+      </c>
+      <c r="B38" t="s">
+        <v>9</v>
+      </c>
+      <c r="C38">
+        <v>2</v>
+      </c>
+      <c r="D38">
+        <v>6</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="F38" t="b">
+        <v>0</v>
+      </c>
+      <c r="G38" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>6</v>
+      </c>
+      <c r="B39" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39">
+        <v>2</v>
+      </c>
+      <c r="D39">
+        <v>7</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39" t="b">
+        <v>0</v>
+      </c>
+      <c r="G39" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>6</v>
+      </c>
+      <c r="B40" t="s">
+        <v>9</v>
+      </c>
+      <c r="C40">
+        <v>2</v>
+      </c>
+      <c r="D40">
+        <v>8</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+      <c r="F40" t="b">
+        <v>0</v>
+      </c>
+      <c r="G40" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>6</v>
+      </c>
+      <c r="B41" t="s">
+        <v>9</v>
+      </c>
+      <c r="C41">
+        <v>2</v>
+      </c>
+      <c r="D41">
+        <v>9</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41" t="b">
+        <v>1</v>
+      </c>
+      <c r="G41" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>6</v>
+      </c>
+      <c r="B42" t="s">
+        <v>7</v>
+      </c>
+      <c r="C42">
+        <v>3</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>6</v>
+      </c>
+      <c r="B43" t="s">
+        <v>7</v>
+      </c>
+      <c r="C43">
+        <v>3</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>6</v>
+      </c>
+      <c r="B44" t="s">
+        <v>7</v>
+      </c>
+      <c r="C44">
+        <v>3</v>
+      </c>
+      <c r="D44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>6</v>
+      </c>
+      <c r="B45" t="s">
+        <v>7</v>
+      </c>
+      <c r="C45">
+        <v>3</v>
+      </c>
+      <c r="D45">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>6</v>
+      </c>
+      <c r="B46" t="s">
+        <v>7</v>
+      </c>
+      <c r="C46">
+        <v>3</v>
+      </c>
+      <c r="D46">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>6</v>
+      </c>
+      <c r="B47" t="s">
+        <v>7</v>
+      </c>
+      <c r="C47">
+        <v>3</v>
+      </c>
+      <c r="D47">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>6</v>
+      </c>
+      <c r="B48" t="s">
+        <v>7</v>
+      </c>
+      <c r="C48">
+        <v>3</v>
+      </c>
+      <c r="D48">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>6</v>
+      </c>
+      <c r="B50" t="s">
+        <v>9</v>
+      </c>
+      <c r="C50">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>6</v>
+      </c>
+      <c r="B51" t="s">
+        <v>9</v>
+      </c>
+      <c r="C51">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>6</v>
+      </c>
+      <c r="B52" t="s">
+        <v>9</v>
+      </c>
+      <c r="C52">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>6</v>
+      </c>
+      <c r="B53" t="s">
+        <v>9</v>
+      </c>
+      <c r="C53">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>6</v>
+      </c>
+      <c r="B54" t="s">
+        <v>9</v>
+      </c>
+      <c r="C54">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>6</v>
+      </c>
+      <c r="B55" t="s">
+        <v>9</v>
+      </c>
+      <c r="C55">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>6</v>
+      </c>
+      <c r="B56" t="s">
+        <v>9</v>
+      </c>
+      <c r="C56">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>6</v>
+      </c>
+      <c r="B57" t="s">
+        <v>9</v>
+      </c>
+      <c r="C57">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>6</v>
+      </c>
+      <c r="B58" t="s">
+        <v>9</v>
+      </c>
+      <c r="C58">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
enter thru AvF 5
</commit_message>
<xml_diff>
--- a/data/cannibalCounts.xlsx
+++ b/data/cannibalCounts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/augkd/Documents/GitHub/forbesiVsrubens/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B9FDF81-1639-CF4D-BAD9-F76B5BDC8262}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14A41F5D-B959-8B4F-B18D-B8673C80DD20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9020" yWindow="500" windowWidth="27640" windowHeight="16940" xr2:uid="{42AF5F07-34B4-EB41-A592-078703C6BD40}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="17">
   <si>
     <t>Experiment</t>
   </si>
@@ -79,17 +79,60 @@
   <si>
     <t>"Cannibalism pileup apparently on non-glower"</t>
   </si>
+  <si>
+    <t>"One big glowing guy. Potential cannibal?"</t>
+  </si>
+  <si>
+    <t>"Non-glowing ossicles spotted"</t>
+  </si>
+  <si>
+    <r>
+      <t>"Non-glower (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>rubens</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) being cannibalized"</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -453,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD071DE8-017B-EB4B-963A-ABFFC1C9D0E0}">
-  <dimension ref="A1:H58"/>
+  <dimension ref="A1:H81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="B86" sqref="B86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1429,6 +1472,15 @@
       <c r="D42">
         <v>0</v>
       </c>
+      <c r="E42">
+        <v>5</v>
+      </c>
+      <c r="F42" t="b">
+        <v>0</v>
+      </c>
+      <c r="G42" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
@@ -1443,6 +1495,15 @@
       <c r="D43">
         <v>1</v>
       </c>
+      <c r="E43">
+        <v>5</v>
+      </c>
+      <c r="F43" t="b">
+        <v>0</v>
+      </c>
+      <c r="G43" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
@@ -1457,6 +1518,15 @@
       <c r="D44">
         <v>2</v>
       </c>
+      <c r="E44">
+        <v>5</v>
+      </c>
+      <c r="F44" t="b">
+        <v>0</v>
+      </c>
+      <c r="G44" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
@@ -1471,6 +1541,18 @@
       <c r="D45">
         <v>3</v>
       </c>
+      <c r="E45">
+        <v>4</v>
+      </c>
+      <c r="F45" t="b">
+        <v>0</v>
+      </c>
+      <c r="G45" t="b">
+        <v>1</v>
+      </c>
+      <c r="H45" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
@@ -1485,6 +1567,15 @@
       <c r="D46">
         <v>4</v>
       </c>
+      <c r="E46">
+        <v>4</v>
+      </c>
+      <c r="F46" t="b">
+        <v>0</v>
+      </c>
+      <c r="G46" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
@@ -1499,6 +1590,15 @@
       <c r="D47">
         <v>5</v>
       </c>
+      <c r="E47">
+        <v>3</v>
+      </c>
+      <c r="F47" t="b">
+        <v>0</v>
+      </c>
+      <c r="G47" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
@@ -1513,19 +1613,63 @@
       <c r="D48">
         <v>6</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E48">
+        <v>3</v>
+      </c>
+      <c r="F48" t="b">
+        <v>0</v>
+      </c>
+      <c r="G48" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>6</v>
+      </c>
+      <c r="B49" t="s">
+        <v>7</v>
+      </c>
+      <c r="C49">
+        <v>3</v>
+      </c>
+      <c r="D49">
+        <v>7</v>
+      </c>
+      <c r="E49">
+        <v>3</v>
+      </c>
+      <c r="F49" t="b">
+        <v>0</v>
+      </c>
+      <c r="G49" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>6</v>
       </c>
       <c r="B50" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C50">
         <v>3</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D50">
+        <v>8</v>
+      </c>
+      <c r="E50">
+        <v>3</v>
+      </c>
+      <c r="F50" t="b">
+        <v>1</v>
+      </c>
+      <c r="G50" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>6</v>
       </c>
@@ -1535,8 +1679,20 @@
       <c r="C51">
         <v>3</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="E51">
+        <v>5</v>
+      </c>
+      <c r="F51" t="b">
+        <v>0</v>
+      </c>
+      <c r="G51" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>6</v>
       </c>
@@ -1546,8 +1702,20 @@
       <c r="C52">
         <v>3</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D52">
+        <v>1</v>
+      </c>
+      <c r="E52">
+        <v>5</v>
+      </c>
+      <c r="F52" t="b">
+        <v>0</v>
+      </c>
+      <c r="G52" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>6</v>
       </c>
@@ -1557,8 +1725,20 @@
       <c r="C53">
         <v>3</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D53">
+        <v>2</v>
+      </c>
+      <c r="E53">
+        <v>4</v>
+      </c>
+      <c r="F53" t="b">
+        <v>0</v>
+      </c>
+      <c r="G53" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>6</v>
       </c>
@@ -1568,8 +1748,20 @@
       <c r="C54">
         <v>3</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D54">
+        <v>3</v>
+      </c>
+      <c r="E54">
+        <v>4</v>
+      </c>
+      <c r="F54" t="b">
+        <v>0</v>
+      </c>
+      <c r="G54" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>6</v>
       </c>
@@ -1579,8 +1771,20 @@
       <c r="C55">
         <v>3</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D55">
+        <v>4</v>
+      </c>
+      <c r="E55">
+        <v>3</v>
+      </c>
+      <c r="F55" t="b">
+        <v>0</v>
+      </c>
+      <c r="G55" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>6</v>
       </c>
@@ -1590,8 +1794,20 @@
       <c r="C56">
         <v>3</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D56">
+        <v>5</v>
+      </c>
+      <c r="E56">
+        <v>3</v>
+      </c>
+      <c r="F56" t="b">
+        <v>0</v>
+      </c>
+      <c r="G56" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>6</v>
       </c>
@@ -1601,8 +1817,20 @@
       <c r="C57">
         <v>3</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D57">
+        <v>6</v>
+      </c>
+      <c r="E57">
+        <v>3</v>
+      </c>
+      <c r="F57" t="b">
+        <v>0</v>
+      </c>
+      <c r="G57" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>6</v>
       </c>
@@ -1611,6 +1839,553 @@
       </c>
       <c r="C58">
         <v>3</v>
+      </c>
+      <c r="D58">
+        <v>7</v>
+      </c>
+      <c r="E58">
+        <v>3</v>
+      </c>
+      <c r="F58" t="b">
+        <v>0</v>
+      </c>
+      <c r="G58" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>6</v>
+      </c>
+      <c r="B59" t="s">
+        <v>9</v>
+      </c>
+      <c r="C59">
+        <v>3</v>
+      </c>
+      <c r="D59">
+        <v>8</v>
+      </c>
+      <c r="E59">
+        <v>3</v>
+      </c>
+      <c r="F59" t="b">
+        <v>1</v>
+      </c>
+      <c r="G59" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>6</v>
+      </c>
+      <c r="B60" t="s">
+        <v>7</v>
+      </c>
+      <c r="C60">
+        <v>4</v>
+      </c>
+      <c r="D60">
+        <v>0</v>
+      </c>
+      <c r="E60">
+        <v>5</v>
+      </c>
+      <c r="F60" t="b">
+        <v>0</v>
+      </c>
+      <c r="G60" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>6</v>
+      </c>
+      <c r="B61" t="s">
+        <v>7</v>
+      </c>
+      <c r="C61">
+        <v>4</v>
+      </c>
+      <c r="D61">
+        <v>1</v>
+      </c>
+      <c r="E61">
+        <v>5</v>
+      </c>
+      <c r="F61" t="b">
+        <v>0</v>
+      </c>
+      <c r="G61" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>6</v>
+      </c>
+      <c r="B62" t="s">
+        <v>7</v>
+      </c>
+      <c r="C62">
+        <v>4</v>
+      </c>
+      <c r="D62">
+        <v>2</v>
+      </c>
+      <c r="E62">
+        <v>5</v>
+      </c>
+      <c r="F62" t="b">
+        <v>0</v>
+      </c>
+      <c r="G62" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>6</v>
+      </c>
+      <c r="B63" t="s">
+        <v>7</v>
+      </c>
+      <c r="C63">
+        <v>4</v>
+      </c>
+      <c r="D63">
+        <v>3</v>
+      </c>
+      <c r="E63">
+        <v>5</v>
+      </c>
+      <c r="F63" t="b">
+        <v>0</v>
+      </c>
+      <c r="G63" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>6</v>
+      </c>
+      <c r="B64" t="s">
+        <v>7</v>
+      </c>
+      <c r="C64">
+        <v>4</v>
+      </c>
+      <c r="D64">
+        <v>4</v>
+      </c>
+      <c r="E64">
+        <v>5</v>
+      </c>
+      <c r="F64" t="b">
+        <v>0</v>
+      </c>
+      <c r="G64" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>6</v>
+      </c>
+      <c r="B65" t="s">
+        <v>7</v>
+      </c>
+      <c r="C65">
+        <v>4</v>
+      </c>
+      <c r="D65">
+        <v>5</v>
+      </c>
+      <c r="E65">
+        <v>5</v>
+      </c>
+      <c r="F65" t="b">
+        <v>1</v>
+      </c>
+      <c r="G65" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>6</v>
+      </c>
+      <c r="B66" t="s">
+        <v>9</v>
+      </c>
+      <c r="C66">
+        <v>4</v>
+      </c>
+      <c r="D66">
+        <v>0</v>
+      </c>
+      <c r="E66">
+        <v>5</v>
+      </c>
+      <c r="F66" t="b">
+        <v>0</v>
+      </c>
+      <c r="G66" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>6</v>
+      </c>
+      <c r="B67" t="s">
+        <v>9</v>
+      </c>
+      <c r="C67">
+        <v>4</v>
+      </c>
+      <c r="D67">
+        <v>1</v>
+      </c>
+      <c r="E67">
+        <v>2</v>
+      </c>
+      <c r="F67" t="b">
+        <v>0</v>
+      </c>
+      <c r="G67" t="b">
+        <v>0</v>
+      </c>
+      <c r="H67" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>6</v>
+      </c>
+      <c r="B68" t="s">
+        <v>9</v>
+      </c>
+      <c r="C68">
+        <v>4</v>
+      </c>
+      <c r="D68">
+        <v>2</v>
+      </c>
+      <c r="E68">
+        <v>0</v>
+      </c>
+      <c r="F68" t="b">
+        <v>0</v>
+      </c>
+      <c r="G68" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>6</v>
+      </c>
+      <c r="B69" t="s">
+        <v>9</v>
+      </c>
+      <c r="C69">
+        <v>4</v>
+      </c>
+      <c r="D69">
+        <v>3</v>
+      </c>
+      <c r="E69">
+        <v>0</v>
+      </c>
+      <c r="F69" t="b">
+        <v>0</v>
+      </c>
+      <c r="G69" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>6</v>
+      </c>
+      <c r="B70" t="s">
+        <v>9</v>
+      </c>
+      <c r="C70">
+        <v>4</v>
+      </c>
+      <c r="D70">
+        <v>4</v>
+      </c>
+      <c r="E70">
+        <v>0</v>
+      </c>
+      <c r="F70" t="b">
+        <v>0</v>
+      </c>
+      <c r="G70" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>6</v>
+      </c>
+      <c r="B71" t="s">
+        <v>9</v>
+      </c>
+      <c r="C71">
+        <v>4</v>
+      </c>
+      <c r="D71">
+        <v>5</v>
+      </c>
+      <c r="E71">
+        <v>0</v>
+      </c>
+      <c r="F71" t="b">
+        <v>1</v>
+      </c>
+      <c r="G71" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>6</v>
+      </c>
+      <c r="B72" t="s">
+        <v>7</v>
+      </c>
+      <c r="C72">
+        <v>5</v>
+      </c>
+      <c r="D72">
+        <v>0</v>
+      </c>
+      <c r="E72">
+        <v>5</v>
+      </c>
+      <c r="F72" t="b">
+        <v>0</v>
+      </c>
+      <c r="G72" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>6</v>
+      </c>
+      <c r="B73" t="s">
+        <v>7</v>
+      </c>
+      <c r="C73">
+        <v>5</v>
+      </c>
+      <c r="D73">
+        <v>1</v>
+      </c>
+      <c r="E73">
+        <v>5</v>
+      </c>
+      <c r="F73" t="b">
+        <v>0</v>
+      </c>
+      <c r="G73" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>6</v>
+      </c>
+      <c r="B74" t="s">
+        <v>7</v>
+      </c>
+      <c r="C74">
+        <v>5</v>
+      </c>
+      <c r="D74">
+        <v>2</v>
+      </c>
+      <c r="E74">
+        <v>4</v>
+      </c>
+      <c r="F74" t="b">
+        <v>0</v>
+      </c>
+      <c r="G74" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>6</v>
+      </c>
+      <c r="B75" t="s">
+        <v>7</v>
+      </c>
+      <c r="C75">
+        <v>5</v>
+      </c>
+      <c r="D75">
+        <v>3</v>
+      </c>
+      <c r="E75">
+        <v>2</v>
+      </c>
+      <c r="F75" t="b">
+        <v>0</v>
+      </c>
+      <c r="G75" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>6</v>
+      </c>
+      <c r="B76" t="s">
+        <v>7</v>
+      </c>
+      <c r="C76">
+        <v>5</v>
+      </c>
+      <c r="D76">
+        <v>4</v>
+      </c>
+      <c r="E76">
+        <v>1</v>
+      </c>
+      <c r="F76" t="b">
+        <v>1</v>
+      </c>
+      <c r="G76" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>6</v>
+      </c>
+      <c r="B77" t="s">
+        <v>9</v>
+      </c>
+      <c r="C77">
+        <v>5</v>
+      </c>
+      <c r="D77">
+        <v>0</v>
+      </c>
+      <c r="E77">
+        <v>5</v>
+      </c>
+      <c r="F77" t="b">
+        <v>0</v>
+      </c>
+      <c r="G77" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>6</v>
+      </c>
+      <c r="B78" t="s">
+        <v>9</v>
+      </c>
+      <c r="C78">
+        <v>5</v>
+      </c>
+      <c r="D78">
+        <v>1</v>
+      </c>
+      <c r="E78">
+        <v>5</v>
+      </c>
+      <c r="F78" t="b">
+        <v>0</v>
+      </c>
+      <c r="G78" t="b">
+        <v>0</v>
+      </c>
+      <c r="H78" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>6</v>
+      </c>
+      <c r="B79" t="s">
+        <v>9</v>
+      </c>
+      <c r="C79">
+        <v>5</v>
+      </c>
+      <c r="D79">
+        <v>2</v>
+      </c>
+      <c r="E79">
+        <v>2</v>
+      </c>
+      <c r="F79" t="b">
+        <v>0</v>
+      </c>
+      <c r="G79" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>6</v>
+      </c>
+      <c r="B80" t="s">
+        <v>9</v>
+      </c>
+      <c r="C80">
+        <v>5</v>
+      </c>
+      <c r="D80">
+        <v>3</v>
+      </c>
+      <c r="E80">
+        <v>1</v>
+      </c>
+      <c r="F80" t="b">
+        <v>0</v>
+      </c>
+      <c r="G80" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>6</v>
+      </c>
+      <c r="B81" t="s">
+        <v>9</v>
+      </c>
+      <c r="C81">
+        <v>5</v>
+      </c>
+      <c r="D81">
+        <v>4</v>
+      </c>
+      <c r="E81">
+        <v>1</v>
+      </c>
+      <c r="F81" t="b">
+        <v>1</v>
+      </c>
+      <c r="G81" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>